<commit_message>
Solved problem with fitness computation and added plot
</commit_message>
<xml_diff>
--- a/JSSP-problems/basic-problem.xlsx
+++ b/JSSP-problems/basic-problem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\URV\Neural-and-Evolutionary-Computation\ACTIVITY2\A2_MarinaLopez\JSSP-problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{816EB42F-74A0-484E-9014-824AAC6E9EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0061BA-82BA-4209-910B-95B038BC1CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10455" yWindow="-18195" windowWidth="32310" windowHeight="15885" xr2:uid="{B0AEE5CE-EC58-4646-B9CB-062555B1B846}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15885" xr2:uid="{B0AEE5CE-EC58-4646-B9CB-062555B1B846}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,8 +37,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -66,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F699FC-FF8C-4F73-9B84-20DB5E8C42DB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>3</v>
       </c>
@@ -421,7 +430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -432,7 +441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -442,6 +451,9 @@
       <c r="C3">
         <v>3</v>
       </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Solved all the problems + added new datasets
</commit_message>
<xml_diff>
--- a/JSSP-problems/basic-problem.xlsx
+++ b/JSSP-problems/basic-problem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\URV\Neural-and-Evolutionary-Computation\ACTIVITY2\A2_MarinaLopez\JSSP-problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0061BA-82BA-4209-910B-95B038BC1CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4925ABAF-1317-43B6-9FD6-324673074CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15885" xr2:uid="{B0AEE5CE-EC58-4646-B9CB-062555B1B846}"/>
+    <workbookView xWindow="11715" yWindow="3420" windowWidth="38700" windowHeight="15885" xr2:uid="{B0AEE5CE-EC58-4646-B9CB-062555B1B846}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,16 +37,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -76,7 +68,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,49 +403,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F699FC-FF8C-4F73-9B84-20DB5E8C42DB}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <v>2</v>
       </c>
       <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>